<commit_message>
trying to find p625 correlation
</commit_message>
<xml_diff>
--- a/data/fifteen_sec_dataset_combined.xlsx
+++ b/data/fifteen_sec_dataset_combined.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="12">
   <si>
     <t>WatchID</t>
   </si>
@@ -49,6 +49,12 @@
     <t>fpdf</t>
   </si>
   <si>
+    <t>Matin  - sanjay</t>
+  </si>
+  <si>
+    <t>Matin / Sanjay</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
 </sst>
@@ -59,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -92,6 +98,11 @@
       <sz val="9"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -214,7 +225,1165 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>MVM</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fifteen_sec_dataset_comparison!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mvm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>fifteen_sec_dataset_comparison!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>8.61634624772928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.64589811500325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.3828990332577</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.58443138520237</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.52284033423879</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.37330761816166</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.1813759836158</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.5602243613911</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.8107417827089</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.1032408900409</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.5891138943856</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.8216415179126</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.5861553966405</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.8486394545185</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.7694339700121</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.4001071184096</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.5765626612099</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.79233524461</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.0122364004194</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.0986934321772</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.8738530805626</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.75165938806811</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.57815966578137</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.54077260289385</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.58229371729561</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.97355964577885</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.2759148795389</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.73520926472744</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.375883448419</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.3073872643831</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.65266707372911</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.76238474260823</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.30298613872564</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.65991914202684</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.35230111299436</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.39489662718069</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.72335690361885</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.32570988843336</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10.0482578745605</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.85148828260121</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9.89244311351117</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.87545718021654</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.74140891033491</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9.92974199275281</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10.1060710551688</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10.2298441772489</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10.046368262461</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10.0436759106415</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.93156420928596</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fifteen_sec_dataset_comparison!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mvm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ed7d31"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>fifteen_sec_dataset_comparison!$K$2:$K$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>8.61634624783078</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.64589811507768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.3828990336398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.58443138541245</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.52284033435477</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.37330761824603</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.1813759838827</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.5602243615213</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.8107417828057</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.1032408901852</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.5891138946711</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.8216415181257</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.586155396692</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.8486394545803</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.7694339700701</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.4001071187612</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.5765626616341</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.7923352451254</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.0122364004846</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.0986934322577</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.87385308064986</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.7516593881523</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.57815966588437</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.5407726029904</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.58229371737259</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.97355964585255</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.27591487968</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.73520926480285</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.375883448777</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.3073872645795</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.65266707378227</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.76238474265376</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.30298613879271</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.6599191420816</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.35230111304838</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.39489662723118</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.72335690366563</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.32570988852323</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10.0482578746681</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.85148828265643</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9.89244311356103</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.87545718027071</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.74140891038357</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9.92974199280129</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10.1060710552883</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10.2298441773145</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10.0463682626599</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10.0436759110302</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.9315642094902</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.76900245189471</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="28661048"/>
+        <c:axId val="17606961"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="28661048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17606961"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="17606961"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="28661048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>SDVM</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fifteen_sec_dataset_comparison!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sdvm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="5b9bd5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>fifteen_sec_dataset_comparison!$D$2:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.0744472794938375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0366053601035815</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.04881663007084</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.74594494256447</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.05014046562698</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0460866271596195</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.59804664072585</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.666236599023526</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81653895511236</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.09015987869883</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.785476038651065</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.560291458102543</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.247392665339913</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.43841589725901</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.963980288567134</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.242850870107914</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.344459343178855</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0834916878053032</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.729831888263328</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.22095169955435</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.307188879314589</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.13294007484976</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.436528019516493</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.369571482530046</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.372923226005803</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.54170549908006</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.226916620653587</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.503217653250256</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.724378224113672</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.436382256506872</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.375097232750935</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.337564830443942</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.358730762868363</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.261065260676175</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.162695294957564</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.0637497125958946</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.463317168322694</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.904597811879099</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.684842732272807</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.0852036040144173</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.0387573318241932</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.151282914309211</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.312902504150404</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.372361790966426</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.16663489709343</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.486901155652241</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.27225391623307</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.0549740515471394</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.762615624277634</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fifteen_sec_dataset_comparison!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sdvm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ed7d31"/>
+            </a:solidFill>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="ed7d31"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>fifteen_sec_dataset_comparison!$L$2:$L$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.0743645142852985</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0365646648636647</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.04765063024848</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.74400392492957</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.04897299394527</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.04603539131583</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5962700459586</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.665495924443168</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.815631185025826</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.08894791622339</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.784602802235114</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.559668565843897</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.247117631712015</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.437928497558043</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.962908603632596</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.242580885896359</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.344076397949972</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0833988676522595</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.729020512914684</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.220706061116494</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.306847368533949</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.132792281513392</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.436042718626652</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.369160619202057</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.372508636400993</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.541103269320975</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.226664350937334</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.502658211530539</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.723572911928403</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.435897117806217</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.374680226248979</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.337189549804219</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.358331951450941</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.260775026826099</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.162514421873431</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.0636788401878483</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.462802085152889</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.903592144187223</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.684081372691903</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.0851088806920097</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.0387142441741871</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.151114728686098</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.312554641328927</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.371947825530238</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.16533791521854</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.486359853479414</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.271951243699172</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.0549129354634171</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.761767802342152</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.259977571482692</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="29247239"/>
+        <c:axId val="725093"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="29247239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="725093"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="725093"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="29247239"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -665,11 +1834,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55485223"/>
-        <c:axId val="30539220"/>
+        <c:axId val="16320580"/>
+        <c:axId val="96222947"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55485223"/>
+        <c:axId val="16320580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,14 +1874,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30539220"/>
+        <c:crossAx val="96222947"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30539220"/>
+        <c:axId val="96222947"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +1924,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55485223"/>
+        <c:crossAx val="16320580"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -793,7 +1962,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1244,11 +2413,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="46926597"/>
-        <c:axId val="1891757"/>
+        <c:axId val="99018781"/>
+        <c:axId val="88347995"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46926597"/>
+        <c:axId val="99018781"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,14 +2453,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1891757"/>
+        <c:crossAx val="88347995"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1891757"/>
+        <c:axId val="88347995"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,7 +2503,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46926597"/>
+        <c:crossAx val="99018781"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1372,7 +2541,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1823,11 +2992,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="71306300"/>
-        <c:axId val="60126235"/>
+        <c:axId val="75487454"/>
+        <c:axId val="4313239"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71306300"/>
+        <c:axId val="75487454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1863,14 +3032,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60126235"/>
+        <c:crossAx val="4313239"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60126235"/>
+        <c:axId val="4313239"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1913,7 +3082,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71306300"/>
+        <c:crossAx val="75487454"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1951,7 +3120,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2402,11 +3571,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="59492488"/>
-        <c:axId val="93411259"/>
+        <c:axId val="93166807"/>
+        <c:axId val="45116942"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59492488"/>
+        <c:axId val="93166807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,14 +3611,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93411259"/>
+        <c:crossAx val="45116942"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93411259"/>
+        <c:axId val="45116942"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2492,7 +3661,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59492488"/>
+        <c:crossAx val="93166807"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2530,7 +3699,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2981,11 +4150,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="24028211"/>
-        <c:axId val="83725383"/>
+        <c:axId val="60121861"/>
+        <c:axId val="61674006"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="24028211"/>
+        <c:axId val="60121861"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3021,14 +4190,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83725383"/>
+        <c:crossAx val="61674006"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83725383"/>
+        <c:axId val="61674006"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3071,1165 +4240,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24028211"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>MVM</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>fifteen_sec_dataset_comparison!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>mvm</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>fifteen_sec_dataset_comparison!$C$2:$C$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>8.61634624772928</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.64589811500325</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.3828990332577</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.58443138520237</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.52284033423879</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.37330761816166</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.1813759836158</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10.5602243613911</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.8107417827089</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.1032408900409</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.5891138943856</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10.8216415179126</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10.5861553966405</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10.8486394545185</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>10.7694339700121</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>10.4001071184096</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10.5765626612099</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10.79233524461</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>10.0122364004194</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10.0986934321772</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.8738530805626</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.75165938806811</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.57815966578137</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.54077260289385</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9.58229371729561</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9.97355964577885</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10.2759148795389</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.73520926472744</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>10.375883448419</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>10.3073872643831</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>9.65266707372911</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.76238474260823</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9.30298613872564</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9.65991914202684</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>9.35230111299436</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>9.39489662718069</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9.72335690361885</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9.32570988843336</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>10.0482578745605</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9.85148828260121</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9.89244311351117</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>9.87545718021654</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>9.74140891033491</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>9.92974199275281</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>10.1060710551688</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>10.2298441772489</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>10.046368262461</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>10.0436759106415</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>9.93156420928596</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>fifteen_sec_dataset_comparison!$K$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>mvm</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ed7d31"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>fifteen_sec_dataset_comparison!$K$2:$K$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>8.61634624783078</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.64589811507768</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.3828990336398</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.58443138541245</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.52284033435477</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.37330761824603</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.1813759838827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10.5602243615213</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.8107417828057</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.1032408901852</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.5891138946711</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10.8216415181257</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10.586155396692</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10.8486394545803</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>10.7694339700701</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>10.4001071187612</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10.5765626616341</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10.7923352451254</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>10.0122364004846</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10.0986934322577</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.87385308064986</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.7516593881523</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.57815966588437</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.5407726029904</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9.58229371737259</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9.97355964585255</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10.27591487968</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.73520926480285</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>10.375883448777</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>10.3073872645795</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>9.65266707378227</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.76238474265376</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9.30298613879271</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9.6599191420816</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>9.35230111304838</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>9.39489662723118</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9.72335690366563</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9.32570988852323</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>10.0482578746681</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9.85148828265643</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9.89244311356103</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>9.87545718027071</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>9.74140891038357</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>9.92974199280129</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>10.1060710552883</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>10.2298441773145</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>10.0463682626599</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>10.0436759110302</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>9.9315642094902</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>8.76900245189471</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="41642185"/>
-        <c:axId val="3890707"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="41642185"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="3890707"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="3890707"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="41642185"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>SDVM</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>fifteen_sec_dataset_comparison!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>sdvm</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>fifteen_sec_dataset_comparison!$D$2:$D$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0.0744472794938375</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0366053601035815</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.04881663007084</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.74594494256447</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.05014046562698</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0460866271596195</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.59804664072585</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.666236599023526</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.81653895511236</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.09015987869883</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.785476038651065</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.560291458102543</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.247392665339913</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.43841589725901</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.963980288567134</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.242850870107914</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.344459343178855</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0834916878053032</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.729831888263328</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.22095169955435</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.307188879314589</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.13294007484976</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.436528019516493</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.369571482530046</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.372923226005803</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.54170549908006</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.226916620653587</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.503217653250256</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.724378224113672</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.436382256506872</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.375097232750935</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.337564830443942</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.358730762868363</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.261065260676175</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.162695294957564</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0637497125958946</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.463317168322694</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.904597811879099</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.684842732272807</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0852036040144173</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0387573318241932</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.151282914309211</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.312902504150404</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.372361790966426</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.16663489709343</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.486901155652241</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.27225391623307</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0549740515471394</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.762615624277634</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>fifteen_sec_dataset_comparison!$L$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>sdvm</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ed7d31"/>
-            </a:solidFill>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>fifteen_sec_dataset_comparison!$L$2:$L$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0.0743645142852985</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0365646648636647</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.04765063024848</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.74400392492957</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.04897299394527</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.04603539131583</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5962700459586</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.665495924443168</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.815631185025826</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.08894791622339</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.784602802235114</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.559668565843897</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.247117631712015</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.437928497558043</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.962908603632596</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.242580885896359</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.344076397949972</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0833988676522595</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.729020512914684</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.220706061116494</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.306847368533949</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.132792281513392</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.436042718626652</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.369160619202057</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.372508636400993</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.541103269320975</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.226664350937334</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.502658211530539</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.723572911928403</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.435897117806217</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.374680226248979</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.337189549804219</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.358331951450941</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.260775026826099</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.162514421873431</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0636788401878483</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.462802085152889</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.903592144187223</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.684081372691903</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0851088806920097</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0387142441741871</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.151114728686098</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.312554641328927</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.371947825530238</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.16533791521854</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.486359853479414</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.271951243699172</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0549129354634171</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.761767802342152</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.259977571482692</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="67789939"/>
-        <c:axId val="66524983"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="67789939"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="66524983"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="66524983"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="67789939"/>
+        <c:crossAx val="60121861"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4272,15 +4283,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>807840</xdr:colOff>
+      <xdr:colOff>835200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>195480</xdr:colOff>
+      <xdr:colOff>222120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>115560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4288,8 +4299,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10409040" y="186120"/>
-        <a:ext cx="4505400" cy="2742840"/>
+        <a:off x="10283760" y="177480"/>
+        <a:ext cx="4425840" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4302,15 +4313,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>788760</xdr:colOff>
+      <xdr:colOff>816120</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>176400</xdr:colOff>
+      <xdr:colOff>203040</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4318,8 +4329,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10389960" y="3024360"/>
-        <a:ext cx="4505400" cy="2743200"/>
+        <a:off x="10264680" y="3015360"/>
+        <a:ext cx="4425840" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4332,15 +4343,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>798120</xdr:colOff>
+      <xdr:colOff>825480</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>185760</xdr:colOff>
+      <xdr:colOff>212400</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4348,8 +4359,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10399320" y="5872680"/>
-        <a:ext cx="4505400" cy="2742840"/>
+        <a:off x="10274040" y="5864040"/>
+        <a:ext cx="4425840" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4362,15 +4373,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>817200</xdr:colOff>
+      <xdr:colOff>844560</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>204840</xdr:colOff>
+      <xdr:colOff>231480</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4378,8 +4389,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10418400" y="8730000"/>
-        <a:ext cx="4505400" cy="2743200"/>
+        <a:off x="10293120" y="8721360"/>
+        <a:ext cx="4425840" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4392,15 +4403,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
+      <xdr:colOff>63360</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>102240</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>340920</xdr:colOff>
+      <xdr:colOff>367560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4408,8 +4419,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="636120" y="10091880"/>
-        <a:ext cx="4505400" cy="2743200"/>
+        <a:off x="653760" y="10083240"/>
+        <a:ext cx="4438080" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4422,15 +4433,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>102240</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>331560</xdr:colOff>
+      <xdr:colOff>358560</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4438,8 +4449,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5427360" y="10091880"/>
-        <a:ext cx="4505400" cy="2743200"/>
+        <a:off x="5369040" y="10083240"/>
+        <a:ext cx="4438080" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4452,15 +4463,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>817200</xdr:colOff>
+      <xdr:colOff>844560</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>204840</xdr:colOff>
+      <xdr:colOff>231480</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>135000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4468,8 +4479,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10418400" y="11597040"/>
-        <a:ext cx="4505400" cy="2742840"/>
+        <a:off x="10293120" y="11588040"/>
+        <a:ext cx="4425840" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4487,17 +4498,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB7" activeCellId="0" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="16" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.265306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4549,10 +4563,16 @@
       <c r="Q1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="Z1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -4598,11 +4618,19 @@
       </c>
       <c r="Q2" s="0" t="n">
         <v>0.0377911239638918</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <f aca="false">G2-O2</f>
+        <v>-0.209675470373626</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <f aca="false">G2/O2</f>
+        <v>0.421794512897444</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -4648,11 +4676,19 @@
       </c>
       <c r="Q3" s="0" t="n">
         <v>0.0575653721182889</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <f aca="false">G3-O3</f>
+        <v>-0.205259312385326</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <f aca="false">G3/O3</f>
+        <v>0.441530768481788</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -4698,11 +4734,19 @@
       </c>
       <c r="Q4" s="0" t="n">
         <v>0.135650085596042</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <f aca="false">G4-O4</f>
+        <v>-0.136459301787439</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <f aca="false">G4/O4</f>
+        <v>0.655724355220965</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -4748,11 +4792,19 @@
       </c>
       <c r="Q5" s="0" t="n">
         <v>0.0626729049359164</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <f aca="false">G5-O5</f>
+        <v>-0.216599192208873</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <f aca="false">G5/O5</f>
+        <v>0.583963514279174</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -4798,11 +4850,19 @@
       </c>
       <c r="Q6" s="0" t="n">
         <v>0.0467817689608687</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <f aca="false">G6-O6</f>
+        <v>-0.272422854247519</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <f aca="false">G6/O6</f>
+        <v>0.504887836822448</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -4848,11 +4908,19 @@
       </c>
       <c r="Q7" s="0" t="n">
         <v>0.124457435496132</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <f aca="false">G7-O7</f>
+        <v>-0.156523535831539</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <f aca="false">G7/O7</f>
+        <v>0.4789742740509</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -4898,11 +4966,19 @@
       </c>
       <c r="Q8" s="0" t="n">
         <v>0.0764498388486416</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <f aca="false">G8-O8</f>
+        <v>-0.158099890964013</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <f aca="false">G8/O8</f>
+        <v>0.62230609748484</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -4948,11 +5024,19 @@
       </c>
       <c r="Q9" s="0" t="n">
         <v>0.0676819921567867</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <f aca="false">G9-O9</f>
+        <v>-0.232098041943884</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <f aca="false">G9/O9</f>
+        <v>0.569567725095514</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>8</v>
@@ -4998,11 +5082,19 @@
       </c>
       <c r="Q10" s="0" t="n">
         <v>0.0494095687797262</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <f aca="false">G10-O10</f>
+        <v>-0.227450101175547</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <f aca="false">G10/O10</f>
+        <v>0.484527045194184</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>9</v>
@@ -5048,11 +5140,19 @@
       </c>
       <c r="Q11" s="0" t="n">
         <v>0.0530248402495444</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <f aca="false">G11-O11</f>
+        <v>-0.290395061451796</v>
+      </c>
+      <c r="AA11" s="0" t="n">
+        <f aca="false">G11/O11</f>
+        <v>0.423016894802964</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>10</v>
@@ -5098,11 +5198,19 @@
       </c>
       <c r="Q12" s="0" t="n">
         <v>0.145459138047153</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <f aca="false">G12-O12</f>
+        <v>-0.133576922046064</v>
+      </c>
+      <c r="AA12" s="0" t="n">
+        <f aca="false">G12/O12</f>
+        <v>0.475356894981836</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>11</v>
@@ -5148,11 +5256,19 @@
       </c>
       <c r="Q13" s="0" t="n">
         <v>0.109707515258131</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <f aca="false">G13-O13</f>
+        <v>-0.169034240870123</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <f aca="false">G13/O13</f>
+        <v>0.484063286919004</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>12</v>
@@ -5198,11 +5314,19 @@
       </c>
       <c r="Q14" s="0" t="n">
         <v>0.0948767363459208</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <f aca="false">G14-O14</f>
+        <v>-0.177369680748268</v>
+      </c>
+      <c r="AA14" s="0" t="n">
+        <f aca="false">G14/O14</f>
+        <v>0.446745485321495</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>13</v>
@@ -5248,11 +5372,19 @@
       </c>
       <c r="Q15" s="0" t="n">
         <v>0.0638900278862375</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <f aca="false">G15-O15</f>
+        <v>-0.273571300024875</v>
+      </c>
+      <c r="AA15" s="0" t="n">
+        <f aca="false">G15/O15</f>
+        <v>0.457546270014188</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>14</v>
@@ -5298,11 +5430,19 @@
       </c>
       <c r="Q16" s="0" t="n">
         <v>0.0620374109341347</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <f aca="false">G16-O16</f>
+        <v>-0.204060268749829</v>
+      </c>
+      <c r="AA16" s="0" t="n">
+        <f aca="false">G16/O16</f>
+        <v>0.639814367018919</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>15</v>
@@ -5348,11 +5488,19 @@
       </c>
       <c r="Q17" s="0" t="n">
         <v>0.0944754724100162</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <f aca="false">G17-O17</f>
+        <v>-0.23559365677412</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <f aca="false">G17/O17</f>
+        <v>0.505592432062918</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>16</v>
@@ -5398,11 +5546,19 @@
       </c>
       <c r="Q18" s="0" t="n">
         <v>0.123300403440974</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <f aca="false">G18-O18</f>
+        <v>-0.150841403289688</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <f aca="false">G18/O18</f>
+        <v>0.656057955860869</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>17</v>
@@ -5448,11 +5604,19 @@
       </c>
       <c r="Q19" s="0" t="n">
         <v>0.0429078185934739</v>
+      </c>
+      <c r="Z19" s="0" t="n">
+        <f aca="false">G19-O19</f>
+        <v>-0.210200908769757</v>
+      </c>
+      <c r="AA19" s="0" t="n">
+        <f aca="false">G19/O19</f>
+        <v>0.447066216988236</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>18</v>
@@ -5498,11 +5662,19 @@
       </c>
       <c r="Q20" s="0" t="n">
         <v>0.051460239140766</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <f aca="false">G20-O20</f>
+        <v>-0.238124649380437</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <f aca="false">G20/O20</f>
+        <v>0.432487569134637</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>19</v>
@@ -5548,11 +5720,19 @@
       </c>
       <c r="Q21" s="0" t="n">
         <v>0.0628300796898404</v>
+      </c>
+      <c r="Z21" s="0" t="n">
+        <f aca="false">G21-O21</f>
+        <v>-0.213742396698671</v>
+      </c>
+      <c r="AA21" s="0" t="n">
+        <f aca="false">G21/O21</f>
+        <v>0.376804671476906</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>20</v>
@@ -5598,11 +5778,19 @@
       </c>
       <c r="Q22" s="0" t="n">
         <v>0.0894966863317258</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <f aca="false">G22-O22</f>
+        <v>-0.178544076549733</v>
+      </c>
+      <c r="AA22" s="0" t="n">
+        <f aca="false">G22/O22</f>
+        <v>0.440785901083006</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>21</v>
@@ -5648,11 +5836,19 @@
       </c>
       <c r="Q23" s="0" t="n">
         <v>0.108218177812966</v>
+      </c>
+      <c r="Z23" s="0" t="n">
+        <f aca="false">G23-O23</f>
+        <v>-0.146094401195743</v>
+      </c>
+      <c r="AA23" s="0" t="n">
+        <f aca="false">G23/O23</f>
+        <v>0.513812487381798</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>22</v>
@@ -5698,11 +5894,19 @@
       </c>
       <c r="Q24" s="0" t="n">
         <v>0.0934881630754491</v>
+      </c>
+      <c r="Z24" s="0" t="n">
+        <f aca="false">G24-O24</f>
+        <v>-0.198888514465644</v>
+      </c>
+      <c r="AA24" s="0" t="n">
+        <f aca="false">G24/O24</f>
+        <v>0.513014011027328</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>23</v>
@@ -5748,11 +5952,19 @@
       </c>
       <c r="Q25" s="0" t="n">
         <v>0.0558274656858018</v>
+      </c>
+      <c r="Z25" s="0" t="n">
+        <f aca="false">G25-O25</f>
+        <v>-0.218582734459546</v>
+      </c>
+      <c r="AA25" s="0" t="n">
+        <f aca="false">G25/O25</f>
+        <v>0.537268622031091</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>24</v>
@@ -5798,11 +6010,19 @@
       </c>
       <c r="Q26" s="0" t="n">
         <v>0.0502815855346934</v>
+      </c>
+      <c r="Z26" s="0" t="n">
+        <f aca="false">G26-O26</f>
+        <v>-0.23502734348329</v>
+      </c>
+      <c r="AA26" s="0" t="n">
+        <f aca="false">G26/O26</f>
+        <v>0.449796253202665</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>25</v>
@@ -5848,11 +6068,19 @@
       </c>
       <c r="Q27" s="0" t="n">
         <v>0.131861224114095</v>
+      </c>
+      <c r="Z27" s="0" t="n">
+        <f aca="false">G27-O27</f>
+        <v>-0.153161306970795</v>
+      </c>
+      <c r="AA27" s="0" t="n">
+        <f aca="false">G27/O27</f>
+        <v>0.450468052579736</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>26</v>
@@ -5898,11 +6126,19 @@
       </c>
       <c r="Q28" s="0" t="n">
         <v>0.0672186749484113</v>
+      </c>
+      <c r="Z28" s="0" t="n">
+        <f aca="false">G28-O28</f>
+        <v>-0.219401375744824</v>
+      </c>
+      <c r="AA28" s="0" t="n">
+        <f aca="false">G28/O28</f>
+        <v>0.452722485116682</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>27</v>
@@ -5948,11 +6184,19 @@
       </c>
       <c r="Q29" s="0" t="n">
         <v>0.070681909716979</v>
+      </c>
+      <c r="Z29" s="0" t="n">
+        <f aca="false">G29-O29</f>
+        <v>-0.21167631502141</v>
+      </c>
+      <c r="AA29" s="0" t="n">
+        <f aca="false">G29/O29</f>
+        <v>0.476679759945871</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>28</v>
@@ -5998,11 +6242,19 @@
       </c>
       <c r="Q30" s="0" t="n">
         <v>0.0928822237069483</v>
+      </c>
+      <c r="Z30" s="0" t="n">
+        <f aca="false">G30-O30</f>
+        <v>-0.191743725716685</v>
+      </c>
+      <c r="AA30" s="0" t="n">
+        <f aca="false">G30/O30</f>
+        <v>0.60937164541537</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>29</v>
@@ -6048,11 +6300,19 @@
       </c>
       <c r="Q31" s="0" t="n">
         <v>0.122347609128189</v>
+      </c>
+      <c r="Z31" s="0" t="n">
+        <f aca="false">G31-O31</f>
+        <v>-0.167634137838604</v>
+      </c>
+      <c r="AA31" s="0" t="n">
+        <f aca="false">G31/O31</f>
+        <v>0.423044995994355</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>30</v>
@@ -6098,11 +6358,19 @@
       </c>
       <c r="Q32" s="0" t="n">
         <v>0.0537167217072707</v>
+      </c>
+      <c r="Z32" s="0" t="n">
+        <f aca="false">G32-O32</f>
+        <v>-0.191073955900965</v>
+      </c>
+      <c r="AA32" s="0" t="n">
+        <f aca="false">G32/O32</f>
+        <v>0.357800243573004</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>31</v>
@@ -6148,11 +6416,19 @@
       </c>
       <c r="Q33" s="0" t="n">
         <v>0.0423507283593537</v>
+      </c>
+      <c r="Z33" s="0" t="n">
+        <f aca="false">G33-O33</f>
+        <v>-0.244730531696015</v>
+      </c>
+      <c r="AA33" s="0" t="n">
+        <f aca="false">G33/O33</f>
+        <v>0.336371991535521</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>32</v>
@@ -6198,11 +6474,19 @@
       </c>
       <c r="Q34" s="0" t="n">
         <v>0.0842898348697074</v>
+      </c>
+      <c r="Z34" s="0" t="n">
+        <f aca="false">G34-O34</f>
+        <v>-0.201866296181607</v>
+      </c>
+      <c r="AA34" s="0" t="n">
+        <f aca="false">G34/O34</f>
+        <v>0.413704030237017</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>33</v>
@@ -6248,11 +6532,19 @@
       </c>
       <c r="Q35" s="0" t="n">
         <v>0.043712896845031</v>
+      </c>
+      <c r="Z35" s="0" t="n">
+        <f aca="false">G35-O35</f>
+        <v>-0.266137207901106</v>
+      </c>
+      <c r="AA35" s="0" t="n">
+        <f aca="false">G35/O35</f>
+        <v>0.433987910964096</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>34</v>
@@ -6298,11 +6590,19 @@
       </c>
       <c r="Q36" s="0" t="n">
         <v>0.0801091765717967</v>
+      </c>
+      <c r="Z36" s="0" t="n">
+        <f aca="false">G36-O36</f>
+        <v>-0.246308311883309</v>
+      </c>
+      <c r="AA36" s="0" t="n">
+        <f aca="false">G36/O36</f>
+        <v>0.511201308700144</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>35</v>
@@ -6348,11 +6648,19 @@
       </c>
       <c r="Q37" s="0" t="n">
         <v>0.0395816786358154</v>
+      </c>
+      <c r="Z37" s="0" t="n">
+        <f aca="false">G37-O37</f>
+        <v>-0.228591720342114</v>
+      </c>
+      <c r="AA37" s="0" t="n">
+        <f aca="false">G37/O37</f>
+        <v>0.512897843197696</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>36</v>
@@ -6398,11 +6706,19 @@
       </c>
       <c r="Q38" s="0" t="n">
         <v>0.0688299968573796</v>
+      </c>
+      <c r="Z38" s="0" t="n">
+        <f aca="false">G38-O38</f>
+        <v>-0.264396691201863</v>
+      </c>
+      <c r="AA38" s="0" t="n">
+        <f aca="false">G38/O38</f>
+        <v>0.382505071222702</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>37</v>
@@ -6448,11 +6764,19 @@
       </c>
       <c r="Q39" s="0" t="n">
         <v>0.086306492838926</v>
+      </c>
+      <c r="Z39" s="0" t="n">
+        <f aca="false">G39-O39</f>
+        <v>-0.200937039011485</v>
+      </c>
+      <c r="AA39" s="0" t="n">
+        <f aca="false">G39/O39</f>
+        <v>0.556054868359615</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>38</v>
@@ -6498,11 +6822,19 @@
       </c>
       <c r="Q40" s="0" t="n">
         <v>0.0420856884404892</v>
+      </c>
+      <c r="Z40" s="0" t="n">
+        <f aca="false">G40-O40</f>
+        <v>-0.200062571534826</v>
+      </c>
+      <c r="AA40" s="0" t="n">
+        <f aca="false">G40/O40</f>
+        <v>0.514953738988577</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>39</v>
@@ -6548,11 +6880,19 @@
       </c>
       <c r="Q41" s="0" t="n">
         <v>0.0447535116248936</v>
+      </c>
+      <c r="Z41" s="0" t="n">
+        <f aca="false">G41-O41</f>
+        <v>-0.235697877877016</v>
+      </c>
+      <c r="AA41" s="0" t="n">
+        <f aca="false">G41/O41</f>
+        <v>0.422509825177313</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>40</v>
@@ -6598,11 +6938,19 @@
       </c>
       <c r="Q42" s="0" t="n">
         <v>0.066552950640639</v>
+      </c>
+      <c r="Z42" s="0" t="n">
+        <f aca="false">G42-O42</f>
+        <v>-0.213773537772664</v>
+      </c>
+      <c r="AA42" s="0" t="n">
+        <f aca="false">G42/O42</f>
+        <v>0.458971190879528</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>41</v>
@@ -6648,11 +6996,19 @@
       </c>
       <c r="Q43" s="0" t="n">
         <v>0.0426165197827203</v>
+      </c>
+      <c r="Z43" s="0" t="n">
+        <f aca="false">G43-O43</f>
+        <v>-0.214440959843137</v>
+      </c>
+      <c r="AA43" s="0" t="n">
+        <f aca="false">G43/O43</f>
+        <v>0.467475212957193</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>42</v>
@@ -6698,11 +7054,19 @@
       </c>
       <c r="Q44" s="0" t="n">
         <v>0.0839147897931143</v>
+      </c>
+      <c r="Z44" s="0" t="n">
+        <f aca="false">G44-O44</f>
+        <v>-0.192444092222121</v>
+      </c>
+      <c r="AA44" s="0" t="n">
+        <f aca="false">G44/O44</f>
+        <v>0.408925086477752</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>43</v>
@@ -6748,11 +7112,19 @@
       </c>
       <c r="Q45" s="0" t="n">
         <v>0.0401967406743995</v>
+      </c>
+      <c r="Z45" s="0" t="n">
+        <f aca="false">G45-O45</f>
+        <v>-0.252976729218696</v>
+      </c>
+      <c r="AA45" s="0" t="n">
+        <f aca="false">G45/O45</f>
+        <v>0.399221349850971</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>44</v>
@@ -6798,11 +7170,19 @@
       </c>
       <c r="Q46" s="0" t="n">
         <v>0.0416459552165367</v>
+      </c>
+      <c r="Z46" s="0" t="n">
+        <f aca="false">G46-O46</f>
+        <v>-0.272164890342935</v>
+      </c>
+      <c r="AA46" s="0" t="n">
+        <f aca="false">G46/O46</f>
+        <v>0.433217350409477</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>45</v>
@@ -6848,11 +7228,19 @@
       </c>
       <c r="Q47" s="0" t="n">
         <v>0.0891188373024735</v>
+      </c>
+      <c r="Z47" s="0" t="n">
+        <f aca="false">G47-O47</f>
+        <v>-0.208522105269981</v>
+      </c>
+      <c r="AA47" s="0" t="n">
+        <f aca="false">G47/O47</f>
+        <v>0.625038586461031</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>46</v>
@@ -6898,11 +7286,19 @@
       </c>
       <c r="Q48" s="0" t="n">
         <v>0.0447914528999327</v>
+      </c>
+      <c r="Z48" s="0" t="n">
+        <f aca="false">G48-O48</f>
+        <v>-0.272858112644317</v>
+      </c>
+      <c r="AA48" s="0" t="n">
+        <f aca="false">G48/O48</f>
+        <v>0.35103138834731</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>47</v>
@@ -6948,11 +7344,19 @@
       </c>
       <c r="Q49" s="0" t="n">
         <v>0.158440482417033</v>
+      </c>
+      <c r="Z49" s="0" t="n">
+        <f aca="false">G49-O49</f>
+        <v>-0.157575409309037</v>
+      </c>
+      <c r="AA49" s="0" t="n">
+        <f aca="false">G49/O49</f>
+        <v>0.525028388743577</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>48</v>
@@ -6998,6 +7402,14 @@
       </c>
       <c r="Q50" s="0" t="n">
         <v>0.160885227447645</v>
+      </c>
+      <c r="Z50" s="0" t="n">
+        <f aca="false">G50-O50</f>
+        <v>-0.166329918711761</v>
+      </c>
+      <c r="AA50" s="0" t="n">
+        <f aca="false">G50/O50</f>
+        <v>0.560767677074003</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7021,6 +7433,14 @@
       </c>
       <c r="Q51" s="0" t="n">
         <v>0.248069440542653</v>
+      </c>
+      <c r="Z51" s="0" t="n">
+        <f aca="false">G51-O51</f>
+        <v>-0.611424409793513</v>
+      </c>
+      <c r="AA51" s="0" t="n">
+        <f aca="false">G51/O51</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>